<commit_message>
Neural Networks - Resultado Final
</commit_message>
<xml_diff>
--- a/Resultado_Neural_Networks_Backup-1.xlsx
+++ b/Resultado_Neural_Networks_Backup-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
   <si>
     <t>lista_funcao_ativacao</t>
   </si>
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,6 +807,88 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>1.208615E-2</v>
+      </c>
+      <c r="E22">
+        <v>2.8101820000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>3.5551069999999997E-2</v>
+      </c>
+      <c r="E23">
+        <v>2.810168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>3.2114980000000001E-2</v>
+      </c>
+      <c r="E25">
+        <v>2.810168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>5.3390029999999998E-2</v>
+      </c>
+      <c r="E26">
+        <v>2.810168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>